<commit_message>
Validate configuration; multiple descriptions; URL regex fix
</commit_message>
<xml_diff>
--- a/spec/fixtures/valid_pqc_descriptive.xlsx
+++ b/spec/fixtures/valid_pqc_descriptive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emeryr/code/GIT/xlsx_to_pqc_xml/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DD3AB8-B408-BF48-A399-ED4D00B13CD8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F5120F-6F4F-0D4F-9AE9-519F0A5DD7C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4000" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
           </rPr>
           <t>Only use when PQC structural metadata spreadsheet is not available.</t>
@@ -73,7 +73,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t>NOTES</t>
   </si>
@@ -285,13 +285,43 @@
   </si>
   <si>
     <t>Other Call number</t>
+  </si>
+  <si>
+    <t>ark:/99999/fk42244n9f</t>
+  </si>
+  <si>
+    <t>Leaf from a book of hours made in France, probably Paris. On the recto and continuing onto the verso is the end of the Gospel reading from Mark, followed by the beginning of the prayer Obsecro te. The beginning of the prayer is marked by the rubric Oratio beate Marie, in red; a 4-line illuminated initial in pink with white penwork on gold grounds, infilled with foliage and flowers; a bar border in gold, blue, and pink on the left edge of the text block; and a three-quarter illuminated border of foliage and ivy on the verso; the recto has no decoration. The text is written in 15 long lines, in Gothic script, and ruled in faint red ink.</t>
+  </si>
+  <si>
+    <t>Ms. Coll. 591</t>
+  </si>
+  <si>
+    <t>Paris, France</t>
+  </si>
+  <si>
+    <t>1 item (1 leaf) : parchment ; 129 x 92 (68 x 43) mm.</t>
+  </si>
+  <si>
+    <t>Latin</t>
+  </si>
+  <si>
+    <t>Sold by King Alfred's Notebook (Cayce, S.C.), cat. 1 (2010), no. 14.</t>
+  </si>
+  <si>
+    <t>http://rightsstatements.org/page/NoC-US/1.0/?</t>
+  </si>
+  <si>
+    <t>Catholic Church|Prayers and devotions - Early works to 1800.|Illumination of books and manuscripts, French |Specimens.</t>
+  </si>
+  <si>
+    <t>Book of hours leaves, ca. 1400.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -308,11 +338,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color indexed="81"/>
@@ -325,6 +350,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -346,13 +382,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -634,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -847,6 +883,44 @@
         <v>56</v>
       </c>
     </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="O3" t="s">
+        <v>66</v>
+      </c>
+      <c r="S3" t="s">
+        <v>67</v>
+      </c>
+      <c r="W3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="Y2" r:id="rId1" xr:uid="{90840819-CC7B-7943-AF05-4A15921E0D70}"/>

</xml_diff>